<commit_message>
set up for second entry
</commit_message>
<xml_diff>
--- a/analysis/species_data/species_list_adding_active.xlsx
+++ b/analysis/species_data/species_list_adding_active.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diaz.renata\Documents\GitHub\BBSsize\analysis\species_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FFA0EE-B044-44B8-872C-3F02F18BCD66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5ABCCB2-329B-41B1-92B4-4A76391CC916}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15375" yWindow="75" windowWidth="15150" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="240" windowWidth="15150" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="species_list" sheetId="1" r:id="rId1"/>
@@ -8911,17 +8911,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U896"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A863" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="J897" sqref="J897"/>
+      <selection pane="bottomLeft" activeCell="C872" sqref="C872"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="7" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>

</xml_diff>